<commit_message>
Changes in most of the modules
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_2.xlsx
+++ b/templates/NHWA_Module_2.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20351"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F9FA6C-1EEE-4F18-B036-72C5F5AC9CC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="/F+XK+b5o34BBpesWDFld7BG994ENQEBkYZjyL564Z/2Z6W0+c/SayrwpqboizQSpvt4drnU3E8HR9PoI7HiAA==" workbookSaltValue="4cbO+hnng67JmnTENcjYug==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA43F887-99FF-414D-AF66-C211CCDDC54E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ga1v+nrD6kb1AGYt8wD/rziE6kym7PE/tdi2hwaN1aQlQHlJf0916PcjCDIPire+kh0X4hlbY7Wz5sppGfMsDQ==" workbookSaltValue="6ijn1QT8HSXyqflHlvqmlw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="Output_Institution" sheetId="2" r:id="rId2"/>
-    <sheet name="Sourcetype" sheetId="4" r:id="rId3"/>
+    <sheet name="Output" sheetId="2" r:id="rId2"/>
+    <sheet name="Institutions" sheetId="5" r:id="rId3"/>
+    <sheet name="Sourcetype" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="dropdownlist">Input!$AE$2:INDEX(Input!$AE$2:$AE$250,MAX(Input!$AD$2:$AD$250),1)</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="805">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2341,25 +2342,10 @@
     <t>Graduates By Gender</t>
   </si>
   <si>
-    <t>Graduates By Institution Ownership</t>
-  </si>
-  <si>
     <t xml:space="preserve">Public </t>
   </si>
   <si>
     <t>Private</t>
-  </si>
-  <si>
-    <t>Educators</t>
-  </si>
-  <si>
-    <t>Education &amp;Training capacity</t>
-  </si>
-  <si>
-    <t>Training Duration</t>
-  </si>
-  <si>
-    <t>Is your master list of accredited education institutions up to date and available in the public domain?</t>
   </si>
   <si>
     <t>YES</t>
@@ -2427,6 +2413,40 @@
   </si>
   <si>
     <t>Other Databases</t>
+  </si>
+  <si>
+    <t>Educators
+(2-05)</t>
+  </si>
+  <si>
+    <t>Education &amp; training capacity (places) (2-03)</t>
+  </si>
+  <si>
+    <t>Training Duration (years) (2-02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        General Paediatricians Practitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Obstetricians and Gynaecologists Practitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Psychiatrists Practitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Medical group of Specialists Practitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Surgical group of Specialists Practitioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Other Specialists Practitioner</t>
+  </si>
+  <si>
+    <t>Is your master list of accredited education institutions up to date and available in the public domain? (2-01)</t>
+  </si>
+  <si>
+    <t>Graduates By Ownership</t>
   </si>
 </sst>
 </file>
@@ -2518,7 +2538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2606,6 +2626,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2630,7 +2676,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -2733,6 +2779,35 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2742,17 +2817,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3002,24 +3080,24 @@
         <xdr:from>
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>7</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4097" name="Drop Down 1" hidden="1">
+            <xdr:cNvPr id="6146" name="Drop Down 2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s4097"/>
+                  <a14:compatExt spid="_x0000_s6146"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3082,7 +3160,7 @@
                   <a14:compatExt spid="_x0000_s1176"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000098040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000098040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3149,7 +3227,7 @@
                   <a14:compatExt spid="_x0000_s1177"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000099040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000099040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3216,7 +3294,7 @@
                   <a14:compatExt spid="_x0000_s1178"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009A040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3283,7 +3361,7 @@
                   <a14:compatExt spid="_x0000_s1179"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009B040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3350,7 +3428,7 @@
                   <a14:compatExt spid="_x0000_s1180"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009C040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3417,7 +3495,7 @@
                   <a14:compatExt spid="_x0000_s1181"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009D040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3484,7 +3562,7 @@
                   <a14:compatExt spid="_x0000_s1182"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009E040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3551,7 +3629,7 @@
                   <a14:compatExt spid="_x0000_s1183"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009F040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00009F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3618,7 +3696,7 @@
                   <a14:compatExt spid="_x0000_s1184"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A0040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A0040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3685,7 +3763,7 @@
                   <a14:compatExt spid="_x0000_s1185"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A1040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A1040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3752,7 +3830,7 @@
                   <a14:compatExt spid="_x0000_s1186"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A2040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A2040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3819,7 +3897,7 @@
                   <a14:compatExt spid="_x0000_s1187"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A3040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A3040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3886,7 +3964,7 @@
                   <a14:compatExt spid="_x0000_s1188"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A4040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A4040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3953,7 +4031,7 @@
                   <a14:compatExt spid="_x0000_s1189"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A5040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000A5040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4020,7 +4098,7 @@
                   <a14:compatExt spid="_x0000_s1197"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AD040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AD040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4087,7 +4165,7 @@
                   <a14:compatExt spid="_x0000_s1198"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AE040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000AE040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4154,7 +4232,7 @@
                   <a14:compatExt spid="_x0000_s1200"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B0040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B0040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4221,7 +4299,7 @@
                   <a14:compatExt spid="_x0000_s1201"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B1040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B1040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4288,7 +4366,7 @@
                   <a14:compatExt spid="_x0000_s1203"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B3040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B3040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4355,7 +4433,7 @@
                   <a14:compatExt spid="_x0000_s1204"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B4040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B4040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4422,7 +4500,7 @@
                   <a14:compatExt spid="_x0000_s1206"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B6040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B6040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4489,7 +4567,7 @@
                   <a14:compatExt spid="_x0000_s1207"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B7040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B7040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4556,7 +4634,7 @@
                   <a14:compatExt spid="_x0000_s1209"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B9040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000B9040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4623,7 +4701,7 @@
                   <a14:compatExt spid="_x0000_s1210"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000BA040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BA040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4690,7 +4768,7 @@
                   <a14:compatExt spid="_x0000_s1212"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000BC040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BC040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4757,7 +4835,7 @@
                   <a14:compatExt spid="_x0000_s1213"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000BD040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BD040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4824,7 +4902,7 @@
                   <a14:compatExt spid="_x0000_s1214"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000BE040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BE040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4891,7 +4969,7 @@
                   <a14:compatExt spid="_x0000_s1215"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000BF040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000BF040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5263,7 +5341,7 @@
   <dimension ref="A1:BZ250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5284,20 +5362,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -5306,7 +5384,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="10" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
@@ -5324,20 +5402,20 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="47" t="s">
         <v>769</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -5509,41 +5587,41 @@
       </c>
     </row>
     <row r="6" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="49" t="s">
         <v>768</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>787</v>
-      </c>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="49" t="s">
+        <v>782</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>779</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49" t="s">
+        <v>783</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>780</v>
+      </c>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49" t="s">
         <v>784</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40" t="s">
-        <v>788</v>
-      </c>
-      <c r="H6" s="40" t="s">
-        <v>785</v>
-      </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40" t="s">
-        <v>789</v>
-      </c>
-      <c r="K6" s="40" t="s">
-        <v>786</v>
-      </c>
-      <c r="L6" s="40"/>
+      <c r="K6" s="49" t="s">
+        <v>781</v>
+      </c>
+      <c r="L6" s="49"/>
       <c r="M6" s="33"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
       <c r="Y6" s="5" t="s">
         <v>18</v>
       </c>
@@ -5570,23 +5648,23 @@
       </c>
     </row>
     <row r="7" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="40"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="40"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="24" t="s">
         <v>11</v>
       </c>
@@ -5680,7 +5758,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -5729,7 +5807,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -12132,7 +12210,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="EHZxZprguYP4sypcsjFl1pnjl29LdkZGqTxZzMvr7MJQg2snXi7ySgR35+PpCb9J25z9FOA24RzyjvpBjzj93w==" saltValue="Btw+Vx5J3hsfUNleH7VT5Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+jikH4mcinbT4Gb/XmZUZu7nnykqlifJmFjJgZE+kN/Gbife06lRlCAktSx3vhVmBNeNrcyIyXLVbbeZKTeOtQ==" saltValue="SEh8NlSuIN5+KAe5fZVSsQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="L4 Q8:R15 M8:P14" name="Range1"/>
     <protectedRange sqref="D8:D11 D13:D14 E8:L14" name="Range1_1"/>
@@ -12150,9 +12228,13 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:L6"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:L14" xr:uid="{E976499E-F417-4AF5-8C43-2FC3834618A6}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{296F17B0-3231-4117-AEFB-F0D82934DBDA}">
+      <formula1>YEAR(TODAY())-20</formula1>
+      <formula2>YEAR(TODAY())-1</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12190,12 +12272,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:U18"/>
+  <dimension ref="B1:U20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:L8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12203,7 +12285,8 @@
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="10.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" style="5" customWidth="1"/>
-    <col min="4" max="14" width="10.7109375" style="5" customWidth="1"/>
+    <col min="4" max="11" width="14.7109375" style="5" customWidth="1"/>
+    <col min="12" max="14" width="10.7109375" style="5" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="5"/>
     <col min="16" max="21" width="9.140625" style="5" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="0" style="5" hidden="1" customWidth="1"/>
@@ -12211,36 +12294,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="47" t="s">
         <v>769</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
       <c r="O2" s="23"/>
       <c r="P2" s="12" t="e">
         <f>Input!V2</f>
@@ -12278,10 +12361,10 @@
         <f>Input!G4</f>
         <v/>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="J4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="28">
+      <c r="K4" s="28">
         <f>Input!L4</f>
         <v>0</v>
       </c>
@@ -12291,40 +12374,46 @@
       <c r="B5" s="6"/>
       <c r="L5" s="6"/>
       <c r="P5" s="12" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>766</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>767</v>
-      </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41" t="s">
-        <v>792</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
+      <c r="C6" s="50" t="s">
+        <v>768</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>791</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49" t="s">
+        <v>804</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49" t="s">
+        <v>789</v>
+      </c>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
       <c r="P6" s="12" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="R6" s="5" t="str">
         <f>IF($P$8=2, "True", "")</f>
@@ -12339,265 +12428,674 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+    <row r="7" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>771</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>772</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>790</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
       <c r="P7" s="12" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="17">
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>777</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
       <c r="P8" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="L9" s="6"/>
+      <c r="B9" s="17">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>785</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="2:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
+    <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="17">
+        <v>4</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>797</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="17">
+        <v>5</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>798</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="17">
+        <v>6</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>799</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="17">
+        <v>7</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>800</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="17">
+        <v>8</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>801</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="17">
         <v>9</v>
       </c>
-      <c r="C10" s="41" t="s">
-        <v>768</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>796</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>770</v>
-      </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40" t="s">
-        <v>771</v>
-      </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="42" t="s">
-        <v>794</v>
-      </c>
-      <c r="J10" s="43"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="40" t="s">
-        <v>774</v>
-      </c>
-      <c r="M10" s="40" t="s">
-        <v>775</v>
-      </c>
-      <c r="N10" s="40" t="s">
-        <v>776</v>
-      </c>
-      <c r="P10" s="12"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="24" t="s">
+      <c r="C16" s="45" t="s">
+        <v>802</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="17">
+        <v>10</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="17">
         <v>11</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="17">
         <v>12</v>
       </c>
-      <c r="G11" s="24" t="s">
-        <v>772</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>773</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>795</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
-        <v>3</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
-        <v>4</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>5</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
-        <v>6</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="C19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
-        <v>7</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="17">
+        <v>13</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/2vJ0Q+woUXAvzoZs3vZhqv8LitmSxg3NkNpPCsdrVI0PXk2w5LPMf1YA/Lju0eAUxcNHUsUTBolV2fXwEPRnw==" saltValue="dggfm6Z/Nv2XLPBbpc1T6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="17">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="F8:L8"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="erWsy34Ypzz/jXwE9S5pRNG/MQdXY1H59b+YGM2GtPJD/E6rmw8VOAu7C71kbHfIlUTu7aCMG1uLpci4zEQLEA==" saltValue="i6TRbk03I38TCpZ9nk99Dg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <mergeCells count="8">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:L7"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:N18" xr:uid="{A3F639C4-71B1-403F-9979-D7791A6DEB32}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:N14" xr:uid="{A3F639C4-71B1-403F-9979-D7791A6DEB32}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587F5560-4E5A-428D-9C1C-242BDFB55787}">
+  <dimension ref="B1:U18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="10.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" style="5" customWidth="1"/>
+    <col min="4" max="6" width="16.7109375" style="5" customWidth="1"/>
+    <col min="7" max="14" width="10.7109375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="5"/>
+    <col min="16" max="21" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+    </row>
+    <row r="2" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="47" t="s">
+        <v>769</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="12" t="e">
+        <f>Input!V2</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28" t="str">
+        <f>Input!V1</f>
+        <v/>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="28" t="str">
+        <f>Input!G4</f>
+        <v/>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="28">
+        <f>Input!L4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="P5" s="12" t="s">
+        <v>773</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>768</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>794</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>796</v>
+      </c>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="P6" s="12" t="s">
+        <v>788</v>
+      </c>
+      <c r="R6" s="5" t="str">
+        <f>IF($P$8=2, "True", "")</f>
+        <v/>
+      </c>
+      <c r="S6" s="5" t="str">
+        <f>IF($P$8=3, "True", "")</f>
+        <v/>
+      </c>
+      <c r="T6" s="5" t="str">
+        <f>IF($P$8=4, "True", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="P7" s="12" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="40">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="P8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="40">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>785</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="40">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="40">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="40">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="40">
+        <v>7</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>766</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>767</v>
+      </c>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50" t="s">
+        <v>787</v>
+      </c>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="50"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+    </row>
+    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="17">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>803</v>
+      </c>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="eeIfyLP+e1FTtxkr/wJ+2jC4GLK76Q7S9rh08pc5H0le3BXH4G048w2nmMKbVSb9cbRNsnO7j0etddlUiqQ1rQ==" saltValue="myLoyL1s9gVu5Frj1i8X9A==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <mergeCells count="13">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F16:J17"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:N14" xr:uid="{3F2DA1F0-36F6-4340-9093-2179365525C9}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -12610,19 +13108,19 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4097" r:id="rId4" name="Drop Down 1">
+            <control shapeId="6146" r:id="rId4" name="Drop Down 2">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>7</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>8</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
@@ -12636,7 +13134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AB50"/>
@@ -12664,15 +13162,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -12682,15 +13180,15 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="2:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
-        <v>782</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="B2" s="47" t="s">
+        <v>777</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -12759,18 +13257,18 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="2:17" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
@@ -12781,19 +13279,19 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="2:17" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="21" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
@@ -12835,7 +13333,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
@@ -12861,7 +13359,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>

</xml_diff>